<commit_message>
updated list and pic
</commit_message>
<xml_diff>
--- a/san.dan.ex.xlsx
+++ b/san.dan.ex.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganmckerlich/Desktop/R.Projects/san dan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganmckerlich/Desktop/R.Projects/SadDan2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6CDCD19-30BC-9D4D-94F7-2C0523B9B537}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55735A67-CC46-D347-BAE8-15484470C907}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3B828615-4E1F-7B46-B5C7-35AAF253EE0F}"/>
   </bookViews>
   <sheets>
-    <sheet name="san.dan" sheetId="1" r:id="rId1"/>
+    <sheet name="san.dan.ex" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>activity</t>
   </si>
@@ -76,6 +76,21 @@
   </si>
   <si>
     <t>desire(1-10)</t>
+  </si>
+  <si>
+    <t>coffee with pau</t>
+  </si>
+  <si>
+    <t>boardwalk run</t>
+  </si>
+  <si>
+    <t>seduce emma</t>
+  </si>
+  <si>
+    <t>see Helen</t>
+  </si>
+  <si>
+    <t>various groundwork</t>
   </si>
 </sst>
 </file>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29D8E1A-61A3-0A40-8FCC-5B5C0F50D29C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +480,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -565,6 +580,61 @@
       </c>
       <c r="C12">
         <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some mormore things to list
</commit_message>
<xml_diff>
--- a/san.dan.ex.xlsx
+++ b/san.dan.ex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganmckerlich/Desktop/R.Projects/SadDan2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E739A77-C405-A14C-9FF9-6823A3A5B53B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886AB78-AE6B-C048-A7F4-305A8E3C1FBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3B828615-4E1F-7B46-B5C7-35AAF253EE0F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>activity</t>
   </si>
@@ -45,9 +45,6 @@
     <t>see brock</t>
   </si>
   <si>
-    <t>go to the beach</t>
-  </si>
-  <si>
     <t>say hey to helens roomates</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>boardwalk run</t>
   </si>
   <si>
-    <t>seduce emma</t>
-  </si>
-  <si>
     <t>see Helen</t>
   </si>
   <si>
@@ -97,6 +91,21 @@
   </si>
   <si>
     <t>garry fiver &amp;dinner</t>
+  </si>
+  <si>
+    <t>seduce emma - connor</t>
+  </si>
+  <si>
+    <t>lay on the beach</t>
+  </si>
+  <si>
+    <t>be in the ocean</t>
+  </si>
+  <si>
+    <t>swim in the pool</t>
+  </si>
+  <si>
+    <t>sunbathe</t>
   </si>
 </sst>
 </file>
@@ -448,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29D8E1A-61A3-0A40-8FCC-5B5C0F50D29C}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -480,18 +489,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -502,7 +511,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -513,7 +522,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -524,7 +533,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -535,7 +544,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -546,7 +555,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -557,7 +566,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -568,7 +577,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -579,7 +588,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -590,7 +599,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -601,7 +610,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -612,7 +621,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -623,7 +632,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -634,7 +643,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -645,7 +654,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -656,13 +665,46 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
title for kable added more variables
</commit_message>
<xml_diff>
--- a/san.dan.ex.xlsx
+++ b/san.dan.ex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganmckerlich/Desktop/R.Projects/SadDan2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886AB78-AE6B-C048-A7F4-305A8E3C1FBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09309A7-820C-6940-A51F-8FAFEC546C36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3B828615-4E1F-7B46-B5C7-35AAF253EE0F}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>that taco place</t>
   </si>
   <si>
-    <t>hype bdm</t>
-  </si>
-  <si>
     <t>see scout</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>get poke</t>
   </si>
   <si>
-    <t>garry fiver &amp;dinner</t>
-  </si>
-  <si>
     <t>seduce emma - connor</t>
   </si>
   <si>
@@ -106,6 +100,12 @@
   </si>
   <si>
     <t>sunbathe</t>
+  </si>
+  <si>
+    <t>garry fiver &amp; dinner</t>
+  </si>
+  <si>
+    <t>beach day monday cali version</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>8</v>

</xml_diff>